<commit_message>
New reports and plots
</commit_message>
<xml_diff>
--- a/reports/Angola_trade_balance_2003-2023.xlsx
+++ b/reports/Angola_trade_balance_2003-2023.xlsx
@@ -846,31 +846,31 @@
         <v>21549256530.51</v>
       </c>
       <c r="C14">
-        <v>18527008742.047</v>
+        <v>18527007950.849</v>
       </c>
       <c r="D14">
         <v>33924937478.31</v>
       </c>
       <c r="E14">
-        <v>36838371233.673</v>
+        <v>36838371246.885</v>
       </c>
       <c r="F14">
         <v>12375680947.8</v>
       </c>
       <c r="G14">
-        <v>15289114703.16301</v>
+        <v>15289114716.375</v>
       </c>
       <c r="H14">
         <v>55474194008.82</v>
       </c>
       <c r="I14">
-        <v>58387627764.183</v>
+        <v>58387627777.395</v>
       </c>
       <c r="J14">
-        <v>1.163126591590795</v>
+        <v>1.16312664126225</v>
       </c>
       <c r="K14">
-        <v>0.9209130681461859</v>
+        <v>0.9209130678159025</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -951,31 +951,31 @@
         <v>16006910579.064</v>
       </c>
       <c r="C17">
-        <v>10345721895.857</v>
+        <v>10345869717.29</v>
       </c>
       <c r="D17">
         <v>40664718814.96</v>
       </c>
       <c r="E17">
-        <v>44190259295.527</v>
+        <v>44190259843.321</v>
       </c>
       <c r="F17">
         <v>24657808235.896</v>
       </c>
       <c r="G17">
-        <v>28183348716.463</v>
+        <v>28183349264.257</v>
       </c>
       <c r="H17">
         <v>56671629394.024</v>
       </c>
       <c r="I17">
-        <v>60197169874.591</v>
+        <v>60197170422.38499</v>
       </c>
       <c r="J17">
-        <v>1.54720093389269</v>
+        <v>1.547178827538615</v>
       </c>
       <c r="K17">
-        <v>0.9202190587525279</v>
+        <v>0.9202190473452521</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -986,31 +986,31 @@
         <v>13961640425.765</v>
       </c>
       <c r="C18">
-        <v>9481649454.854</v>
+        <v>9485654695.275999</v>
       </c>
       <c r="D18">
         <v>35432454858.832</v>
       </c>
       <c r="E18">
-        <v>37542311664.656</v>
+        <v>37542603376.893</v>
       </c>
       <c r="F18">
         <v>21470814433.067</v>
       </c>
       <c r="G18">
-        <v>23580671238.891</v>
+        <v>23580962951.128</v>
       </c>
       <c r="H18">
         <v>49394095284.597</v>
       </c>
       <c r="I18">
-        <v>51503952090.421</v>
+        <v>51504243802.658</v>
       </c>
       <c r="J18">
-        <v>1.472490677096012</v>
+        <v>1.471868929902973</v>
       </c>
       <c r="K18">
-        <v>0.9438005622916846</v>
+        <v>0.9437932288052308</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1021,31 +1021,31 @@
         <v>9337925708.641001</v>
       </c>
       <c r="C19">
-        <v>7579164285.011</v>
+        <v>7578675569.81</v>
       </c>
       <c r="D19">
         <v>22134505473.377</v>
       </c>
       <c r="E19">
-        <v>24012461247.855</v>
+        <v>24012465084.335</v>
       </c>
       <c r="F19">
         <v>12796579764.736</v>
       </c>
       <c r="G19">
-        <v>14674535539.214</v>
+        <v>14674539375.694</v>
       </c>
       <c r="H19">
         <v>31472431182.018</v>
       </c>
       <c r="I19">
-        <v>33350386956.496</v>
+        <v>33350390792.976</v>
       </c>
       <c r="J19">
-        <v>1.23205215740055</v>
+        <v>1.232131606984082</v>
       </c>
       <c r="K19">
-        <v>0.9217924495496789</v>
+        <v>0.9217923022745748</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1056,31 +1056,31 @@
         <v>11378927920.701</v>
       </c>
       <c r="C20">
-        <v>9449572419.052</v>
+        <v>9447401489.256001</v>
       </c>
       <c r="D20">
         <v>34472161956.832</v>
       </c>
       <c r="E20">
-        <v>33645511738.133</v>
+        <v>33624563124.17</v>
       </c>
       <c r="F20">
         <v>23093234036.131</v>
       </c>
       <c r="G20">
-        <v>22266583817.432</v>
+        <v>22245635203.469</v>
       </c>
       <c r="H20">
         <v>45851089877.533</v>
       </c>
       <c r="I20">
-        <v>45024439658.834</v>
+        <v>45003491044.871</v>
       </c>
       <c r="J20">
-        <v>1.204173841533727</v>
+        <v>1.204450550094819</v>
       </c>
       <c r="K20">
-        <v>1.024569405427176</v>
+        <v>1.025207727741531</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1091,31 +1091,31 @@
         <v>17802935241.948</v>
       </c>
       <c r="C21">
-        <v>14267672182.795</v>
+        <v>14260494508.633</v>
       </c>
       <c r="D21">
         <v>51274951711.647</v>
       </c>
       <c r="E21">
-        <v>52943571614.454</v>
+        <v>52905676359.56</v>
       </c>
       <c r="F21">
         <v>33472016469.699</v>
       </c>
       <c r="G21">
-        <v>35140636372.506</v>
+        <v>35102741117.612</v>
       </c>
       <c r="H21">
         <v>69077886953.595</v>
       </c>
       <c r="I21">
-        <v>70746506856.40201</v>
+        <v>70708611601.508</v>
       </c>
       <c r="J21">
-        <v>1.247781348902597</v>
+        <v>1.248409389391825</v>
       </c>
       <c r="K21">
-        <v>0.9684830499355382</v>
+        <v>0.9691767545540825</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1123,16 +1123,16 @@
         <v>31</v>
       </c>
       <c r="C22">
-        <v>10812915513.618</v>
+        <v>9152383958.514</v>
       </c>
       <c r="E22">
-        <v>35312785387.256</v>
+        <v>25988479965.46</v>
       </c>
       <c r="G22">
-        <v>35312785387.256</v>
+        <v>25988479965.46</v>
       </c>
       <c r="I22">
-        <v>35312785387.256</v>
+        <v>25988479965.46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>